<commit_message>
Versione finale per export (commentato via GRASP temporaneamente)
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/errori_tassative.xlsx
+++ b/PS-VRP/Dati_output/errori_tassative.xlsx
@@ -442,23 +442,23 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251231</v>
+        <v>252277</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45846.58333333334</v>
+        <v>45847.58333333334</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>252277</v>
+        <v>251849</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>45847.58333333334</v>
+        <v>45846.58333333334</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251849</v>
+        <v>251231</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45846.58333333334</v>

</xml_diff>

<commit_message>
Tentativo correzione problema commesse identiche non attaccate #1
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/errori_tassative.xlsx
+++ b/PS-VRP/Dati_output/errori_tassative.xlsx
@@ -442,23 +442,23 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251231</v>
+        <v>252277</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45846.58333333334</v>
+        <v>45847.58333333334</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>252277</v>
+        <v>251849</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>45847.58333333334</v>
+        <v>45846.58333333334</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251849</v>
+        <v>251231</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45846.58333333334</v>

</xml_diff>

<commit_message>
Non si capisce più nulla
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/errori_tassative.xlsx
+++ b/PS-VRP/Dati_output/errori_tassative.xlsx
@@ -442,18 +442,18 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251849</v>
+        <v>252277</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45846.58333333334</v>
+        <v>45847.58333333334</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>252277</v>
+        <v>251849</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>45847.58333333334</v>
+        <v>45846.58333333334</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Ultima versione del giorno, introdotto il "divid"
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/errori_tassative.xlsx
+++ b/PS-VRP/Dati_output/errori_tassative.xlsx
@@ -442,15 +442,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>252277</v>
+        <v>251849</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45847.58333333334</v>
+        <v>45846.58333333334</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251849</v>
+        <v>252284</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>45846.58333333334</v>
@@ -458,7 +458,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>252284</v>
+        <v>251231</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45846.58333333334</v>
@@ -466,10 +466,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251231</v>
+        <v>252277</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>45846.58333333334</v>
+        <v>45847.58333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>